<commit_message>
Continuação da construção da planilha de valores
</commit_message>
<xml_diff>
--- a/docs/projeto-final/documento-final/pesquisas/acompanhamento-valores.xlsx
+++ b/docs/projeto-final/documento-final/pesquisas/acompanhamento-valores.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desenvolvimento\FAI\fai.etanois.docs\docs\projeto-final\documento-final\pesquisas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.barbosa\Desktop\SM\Outros\fai.etanois.docs\docs\projeto-final\documento-final\pesquisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20469E7-E529-4014-BD21-C2DA85FC1805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C29B3FB-47FE-454D-9F3C-8625AB644A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -66,7 +64,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.000;[Red]\-&quot;R$&quot;\ #,##0.000"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,14 +102,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -113,6 +139,1441 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avenida II</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43851</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$C$5:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.859</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6180-4739-801B-3BC4BBF5FA79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brusamolin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43851</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$C$6:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>5.0890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6180-4739-801B-3BC4BBF5FA79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Combo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43851</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$C$7:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="3">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6180-4739-801B-3BC4BBF5FA79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43851</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$C$8:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.000;[Red]\-&quot;R$&quot;\ #,##0.000">
+                  <c:v>5.149</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6180-4739-801B-3BC4BBF5FA79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sêda</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43851</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$C$9:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6180-4739-801B-3BC4BBF5FA79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zezão</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43851</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$C$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.1390000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1390000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1390000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1390000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1390000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6180-4739-801B-3BC4BBF5FA79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="479536272"/>
+        <c:axId val="479537584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="479536272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479537584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="479537584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.2"/>
+          <c:min val="4.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479536272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>151499</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>137437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25E3CE3B-7367-403B-88F0-7E7FD6B2B7ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,84 +1873,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F419A0E-6C88-4CD1-BCBF-61ABD01E164E}">
-  <dimension ref="B2:I10"/>
+  <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="1"/>
+    <col min="2" max="6" width="20.7109375" style="1" customWidth="1"/>
+    <col min="7" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="2.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>43836</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>43837</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
+        <v>43839</v>
+      </c>
+      <c r="F4" s="2">
         <v>43840</v>
       </c>
-      <c r="F4" s="1">
-        <v>43839</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>43844</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>43845</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
         <v>43851</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4.859</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4.859</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4.859</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4.859</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.859</v>
+      </c>
+      <c r="H5" s="4">
+        <v>4.859</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4.859</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <v>5.0890000000000004</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5.0890000000000004</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.0890000000000004</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5.1589999999999998</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5.1589999999999998</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5.1589999999999998</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="H7" s="4">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="I7" s="4">
+        <v>4.9489999999999998</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4">
+        <v>5.149</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5.1989999999999998</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5.1989999999999998</v>
+      </c>
+      <c r="G8" s="4">
+        <v>5.1989999999999998</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5.1989999999999998</v>
+      </c>
+      <c r="I8" s="3">
+        <v>5.149</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C10" s="4">
+        <v>5.1390000000000002</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5.1390000000000002</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5.1390000000000002</v>
+      </c>
+      <c r="F10" s="4">
+        <v>5.1390000000000002</v>
+      </c>
+      <c r="G10" s="4">
+        <v>5.1390000000000002</v>
+      </c>
+      <c r="H10" s="4">
+        <v>5.1589999999999998</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5.1589999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Término do preenchimento dos valores de Gasolina e Etanol em Santa Rita. Falta fechamento do dia 06/03/2020
</commit_message>
<xml_diff>
--- a/docs/projeto-final/documento-final/pesquisas/acompanhamento-valores.xlsx
+++ b/docs/projeto-final/documento-final/pesquisas/acompanhamento-valores.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.barbosa\Desktop\SM\Outros\fai.etanois.docs\docs\projeto-final\documento-final\pesquisas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desenvolvimento\FAI\fai.etanois.docs\docs\projeto-final\documento-final\pesquisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C29B3FB-47FE-454D-9F3C-8625AB644A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7668F2-6E30-40B8-8A02-433F9A735C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pesquisa #01" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Pesquisa #01 - Acompanhamento dos valores dos postos de combustível</t>
   </si>
@@ -42,31 +42,36 @@
     <t>Santa Rita do Sapucaí, MG</t>
   </si>
   <si>
-    <t>Avenida II</t>
+    <t>Avenida II (Branca)</t>
   </si>
   <si>
-    <t>Brusamolin</t>
+    <t>Brusamolin (BR)</t>
   </si>
   <si>
-    <t>Combo</t>
+    <t>Combo (Branca)</t>
   </si>
   <si>
-    <t>Shell</t>
+    <t>Shell (Shell)</t>
   </si>
   <si>
-    <t>Sêda</t>
+    <t>Sêda (Branca)</t>
   </si>
   <si>
-    <t>Zezão</t>
+    <t>Zezão (BR)</t>
+  </si>
+  <si>
+    <t>Gasolina Comum</t>
+  </si>
+  <si>
+    <t>Etanol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.000;[Red]\-&quot;R$&quot;\ #,##0.000"/>
     <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -106,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -114,13 +119,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -156,6 +177,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Valores da Gasolina Comum</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> em Santa Rita do Sapucaí-MG entre 06/01/2020 e 06/03/2020</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -196,11 +247,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$5</c:f>
+              <c:f>'Pesquisa #01'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avenida II</c:v>
+                  <c:v>Avenida II (Branca)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -231,10 +282,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:f>'Pesquisa #01'!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
                 </c:pt>
@@ -255,16 +306,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43851</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$5:$I$5</c:f>
+              <c:f>'Pesquisa #01'!$C$6:$Q$6</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>4.859</c:v>
                 </c:pt>
@@ -284,6 +359,27 @@
                   <c:v>4.859</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.859</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>4.859</c:v>
                 </c:pt>
               </c:numCache>
@@ -292,7 +388,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6180-4739-801B-3BC4BBF5FA79}"/>
+              <c16:uniqueId val="{00000000-4671-4359-9B29-6799C65EB26A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -301,11 +397,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$6</c:f>
+              <c:f>'Pesquisa #01'!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Brusamolin</c:v>
+                  <c:v>Brusamolin (BR)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -336,10 +432,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:f>'Pesquisa #01'!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
                 </c:pt>
@@ -360,16 +456,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43851</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$6:$I$6</c:f>
+              <c:f>'Pesquisa #01'!$C$7:$Q$7</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="1">
                   <c:v>5.0890000000000004</c:v>
                 </c:pt>
@@ -387,6 +507,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0789999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,7 +535,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6180-4739-801B-3BC4BBF5FA79}"/>
+              <c16:uniqueId val="{00000001-4671-4359-9B29-6799C65EB26A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -403,11 +544,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$7</c:f>
+              <c:f>'Pesquisa #01'!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Combo</c:v>
+                  <c:v>Combo (Branca)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -438,10 +579,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:f>'Pesquisa #01'!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
                 </c:pt>
@@ -462,16 +603,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43851</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$7:$I$7</c:f>
+              <c:f>'Pesquisa #01'!$C$8:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="3">
                   <c:v>4.9489999999999998</c:v>
                 </c:pt>
@@ -482,6 +647,30 @@
                   <c:v>4.9489999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>4.9489999999999998</c:v>
                 </c:pt>
               </c:numCache>
@@ -490,7 +679,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6180-4739-801B-3BC4BBF5FA79}"/>
+              <c16:uniqueId val="{00000002-4671-4359-9B29-6799C65EB26A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -499,11 +688,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$8</c:f>
+              <c:f>'Pesquisa #01'!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Shell</c:v>
+                  <c:v>Shell (Shell)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -534,10 +723,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:f>'Pesquisa #01'!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
                 </c:pt>
@@ -558,16 +747,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43851</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$8:$I$8</c:f>
+              <c:f>'Pesquisa #01'!$C$9:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="1">
                   <c:v>5.149</c:v>
                 </c:pt>
@@ -583,8 +796,29 @@
                 <c:pt idx="5">
                   <c:v>5.1989999999999998</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.000;[Red]\-&quot;R$&quot;\ #,##0.000">
+                <c:pt idx="6">
                   <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0490000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0490000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -592,7 +826,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6180-4739-801B-3BC4BBF5FA79}"/>
+              <c16:uniqueId val="{00000003-4671-4359-9B29-6799C65EB26A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -601,11 +835,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$9</c:f>
+              <c:f>'Pesquisa #01'!$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sêda</c:v>
+                  <c:v>Sêda (Branca)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -636,10 +870,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:f>'Pesquisa #01'!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
                 </c:pt>
@@ -660,23 +894,71 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43851</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$9:$I$9</c:f>
+              <c:f>'Pesquisa #01'!$C$10:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
+                <c:pt idx="7">
+                  <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.1989999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-6180-4739-801B-3BC4BBF5FA79}"/>
+              <c16:uniqueId val="{00000004-4671-4359-9B29-6799C65EB26A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -685,11 +967,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$B$10</c:f>
+              <c:f>'Pesquisa #01'!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Zezão</c:v>
+                  <c:v>Zezão (BR)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -720,10 +1002,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$I$4</c:f>
+              <c:f>'Pesquisa #01'!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
                 </c:pt>
@@ -744,16 +1026,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43851</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$10:$I$10</c:f>
+              <c:f>'Pesquisa #01'!$C$11:$Q$11</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>5.1390000000000002</c:v>
                 </c:pt>
@@ -774,6 +1080,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.149</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0590000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,12 +1108,11 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-6180-4739-801B-3BC4BBF5FA79}"/>
+              <c16:uniqueId val="{00000005-4671-4359-9B29-6799C65EB26A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -796,11 +1122,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="479536272"/>
-        <c:axId val="479537584"/>
+        <c:axId val="1669594240"/>
+        <c:axId val="1669464176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="479536272"/>
+        <c:axId val="1669594240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,7 +1169,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479537584"/>
+        <c:crossAx val="1669464176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -851,7 +1177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479537584"/>
+        <c:axId val="1669464176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.2"/>
@@ -904,10 +1230,1085 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479536272"/>
+        <c:crossAx val="1669594240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Valores do Etanol em Santa Rita do Sapucaí-MG entre 06/01/2020 e 06/03/2020</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pesquisa #01'!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avenida II (Branca)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$14:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$15:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="1">
+                  <c:v>3.359</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.359</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.359</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.359</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.359</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.359</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.359</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.399</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.399</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C35-443A-ACE1-5EA6B21FF31F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pesquisa #01'!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brusamolin (BR)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$14:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$16:$O$16</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="1">
+                  <c:v>3.4590000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4590000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4590000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.669</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.669</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.669</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.669</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8C35-443A-ACE1-5EA6B21FF31F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pesquisa #01'!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Combo (Branca)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$14:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$17:$O$17</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="3">
+                  <c:v>3.4590000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3889999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3889999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.3889999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8C35-443A-ACE1-5EA6B21FF31F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pesquisa #01'!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell (Shell)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$14:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$18:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="1">
+                  <c:v>3.4990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8C35-443A-ACE1-5EA6B21FF31F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pesquisa #01'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sêda (Branca)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$14:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$19:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="6">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8C35-443A-ACE1-5EA6B21FF31F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pesquisa #01'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zezão (BR)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$14:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pesquisa #01'!$C$20:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.5190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.7690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6589999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8C35-443A-ACE1-5EA6B21FF31F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1848667776"/>
+        <c:axId val="1667319408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1848667776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1667319408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1667319408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.8"/>
+          <c:min val="3.3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1848667776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1032,8 +2433,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1141,6 +2582,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1151,6 +2597,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1182,6 +2633,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1535,27 +2989,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>173180</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>230330</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>151499</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>137437</xdr:rowOff>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>99544</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>53875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Gráfico 9">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25E3CE3B-7367-403B-88F0-7E7FD6B2B7ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D84F5650-C85E-4159-8742-2196B70611FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1568,6 +3525,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>17318</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>5194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>116863</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>71194</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D42BCD72-D796-4996-82A1-9088FE4F815C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1873,189 +3866,865 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F419A0E-6C88-4CD1-BCBF-61ABD01E164E}">
-  <dimension ref="B2:I11"/>
+  <dimension ref="B2:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="CO25" sqref="CO25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="1"/>
-    <col min="2" max="6" width="20.7109375" style="1" customWidth="1"/>
-    <col min="7" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="2.7109375" style="1"/>
+    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="3" max="17" width="15.7109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="2.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>43836</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="2">
         <v>43837</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E5" s="2">
         <v>43839</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <v>43840</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G5" s="2">
         <v>43844</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H5" s="2">
         <v>43845</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I5" s="2">
         <v>43851</v>
       </c>
+      <c r="J5" s="2">
+        <v>43864</v>
+      </c>
+      <c r="K5" s="2">
+        <v>43871</v>
+      </c>
+      <c r="L5" s="2">
+        <v>43873</v>
+      </c>
+      <c r="M5" s="2">
+        <v>43874</v>
+      </c>
+      <c r="N5" s="2">
+        <v>43882</v>
+      </c>
+      <c r="O5" s="2">
+        <v>43889</v>
+      </c>
+      <c r="P5" s="2">
+        <v>43894</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>43896</v>
+      </c>
     </row>
-    <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="3">
         <v>4.859</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="3">
         <v>4.859</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="3">
         <v>4.859</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="3">
         <v>4.859</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G6" s="3">
         <v>4.859</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H6" s="3">
         <v>4.859</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I6" s="3">
         <v>4.859</v>
       </c>
+      <c r="J6" s="3">
+        <v>4.859</v>
+      </c>
+      <c r="K6" s="3">
+        <v>4.859</v>
+      </c>
+      <c r="L6" s="3">
+        <v>4.859</v>
+      </c>
+      <c r="M6" s="3">
+        <v>4.859</v>
+      </c>
+      <c r="N6" s="3">
+        <v>4.859</v>
+      </c>
+      <c r="O6" s="3">
+        <v>4.859</v>
+      </c>
+      <c r="P6" s="3">
+        <v>4.859</v>
+      </c>
     </row>
-    <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
         <v>5.0890000000000004</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E7" s="3">
         <v>5.0890000000000004</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F7" s="3">
         <v>5.0890000000000004</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G7" s="3">
         <v>5.1589999999999998</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H7" s="3">
         <v>5.1589999999999998</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I7" s="3">
         <v>5.1589999999999998</v>
       </c>
+      <c r="J7" s="3">
+        <v>5.1589999999999998</v>
+      </c>
+      <c r="K7" s="3">
+        <v>5.1589999999999998</v>
+      </c>
+      <c r="L7" s="3">
+        <v>5.1589999999999998</v>
+      </c>
+      <c r="M7" s="3">
+        <v>5.0789999999999997</v>
+      </c>
+      <c r="N7" s="3">
+        <v>5.0789999999999997</v>
+      </c>
+      <c r="O7" s="3">
+        <v>5.0789999999999997</v>
+      </c>
+      <c r="P7" s="3">
+        <v>5.0789999999999997</v>
+      </c>
     </row>
-    <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
         <v>4.9489999999999998</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G8" s="3">
         <v>4.9489999999999998</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H8" s="3">
         <v>4.9489999999999998</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I8" s="3">
         <v>4.9489999999999998</v>
       </c>
+      <c r="J8" s="3">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="L8" s="3">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="M8" s="3">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="N8" s="3">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="O8" s="3">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="P8" s="3">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>4.9489999999999998</v>
+      </c>
     </row>
-    <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
         <v>5.149</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E9" s="3">
         <v>5.1989999999999998</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F9" s="3">
         <v>5.1989999999999998</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G9" s="3">
         <v>5.1989999999999998</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H9" s="3">
         <v>5.1989999999999998</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I9" s="3">
         <v>5.149</v>
       </c>
+      <c r="J9" s="3">
+        <v>5.149</v>
+      </c>
+      <c r="K9" s="3">
+        <v>5.149</v>
+      </c>
+      <c r="L9" s="3">
+        <v>5.0990000000000002</v>
+      </c>
+      <c r="M9" s="3">
+        <v>5.0990000000000002</v>
+      </c>
+      <c r="N9" s="3">
+        <v>5.149</v>
+      </c>
+      <c r="O9" s="3">
+        <v>5.0490000000000004</v>
+      </c>
+      <c r="P9" s="3">
+        <v>5.0490000000000004</v>
+      </c>
     </row>
-    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="J10" s="3">
+        <v>5.149</v>
+      </c>
+      <c r="K10" s="3">
+        <v>5.149</v>
+      </c>
+      <c r="L10" s="3">
+        <v>5.0990000000000002</v>
+      </c>
+      <c r="M10" s="3">
+        <v>5.0990000000000002</v>
+      </c>
+      <c r="N10" s="3">
+        <v>5.0990000000000002</v>
+      </c>
+      <c r="O10" s="3">
+        <v>5.0990000000000002</v>
+      </c>
+      <c r="P10" s="3">
+        <v>5.0990000000000002</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>5.1989999999999998</v>
+      </c>
     </row>
-    <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="3">
         <v>5.1390000000000002</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D11" s="3">
         <v>5.1390000000000002</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E11" s="3">
         <v>5.1390000000000002</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F11" s="3">
         <v>5.1390000000000002</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G11" s="3">
         <v>5.1390000000000002</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H11" s="3">
         <v>5.1589999999999998</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I11" s="3">
         <v>5.1589999999999998</v>
       </c>
+      <c r="J11" s="3">
+        <v>5.1589999999999998</v>
+      </c>
+      <c r="K11" s="3">
+        <v>5.0789999999999997</v>
+      </c>
+      <c r="L11" s="3">
+        <v>5.0789999999999997</v>
+      </c>
+      <c r="M11" s="3">
+        <v>5.0789999999999997</v>
+      </c>
+      <c r="N11" s="3">
+        <v>5.149</v>
+      </c>
+      <c r="O11" s="3">
+        <v>5.149</v>
+      </c>
+      <c r="P11" s="3">
+        <v>5.0590000000000002</v>
+      </c>
     </row>
-    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="4"/>
+    <row r="13" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>43836</v>
+      </c>
+      <c r="D14" s="8">
+        <v>43837</v>
+      </c>
+      <c r="E14" s="8">
+        <v>43839</v>
+      </c>
+      <c r="F14" s="8">
+        <v>43840</v>
+      </c>
+      <c r="G14" s="8">
+        <v>43844</v>
+      </c>
+      <c r="H14" s="8">
+        <v>43845</v>
+      </c>
+      <c r="I14" s="8">
+        <v>43864</v>
+      </c>
+      <c r="J14" s="8">
+        <v>43874</v>
+      </c>
+      <c r="K14" s="8">
+        <v>43881</v>
+      </c>
+      <c r="L14" s="8">
+        <v>43882</v>
+      </c>
+      <c r="M14" s="8">
+        <v>43888</v>
+      </c>
+      <c r="N14" s="8">
+        <v>43894</v>
+      </c>
+      <c r="O14" s="8">
+        <v>43896</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10">
+        <v>3.359</v>
+      </c>
+      <c r="E15" s="10">
+        <v>3.359</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3.359</v>
+      </c>
+      <c r="G15" s="10">
+        <v>3.359</v>
+      </c>
+      <c r="H15" s="10">
+        <v>3.359</v>
+      </c>
+      <c r="I15" s="10">
+        <v>3.359</v>
+      </c>
+      <c r="J15" s="10">
+        <v>3.359</v>
+      </c>
+      <c r="K15" s="10">
+        <v>3.399</v>
+      </c>
+      <c r="L15" s="10">
+        <v>3.399</v>
+      </c>
+      <c r="M15" s="10">
+        <v>3.399</v>
+      </c>
+      <c r="N15" s="10">
+        <v>3.399</v>
+      </c>
+      <c r="O15" s="11"/>
+    </row>
+    <row r="16" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10">
+        <v>3.4590000000000001</v>
+      </c>
+      <c r="E16" s="10">
+        <v>3.4590000000000001</v>
+      </c>
+      <c r="F16" s="10">
+        <v>3.4590000000000001</v>
+      </c>
+      <c r="G16" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="H16" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="I16" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="J16" s="10">
+        <v>3.669</v>
+      </c>
+      <c r="K16" s="10">
+        <v>3.669</v>
+      </c>
+      <c r="L16" s="10">
+        <v>3.669</v>
+      </c>
+      <c r="M16" s="10">
+        <v>3.669</v>
+      </c>
+      <c r="N16" s="10">
+        <v>3.669</v>
+      </c>
+      <c r="O16" s="11"/>
+    </row>
+    <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10">
+        <v>3.4590000000000001</v>
+      </c>
+      <c r="G17" s="10">
+        <v>3.3490000000000002</v>
+      </c>
+      <c r="H17" s="10">
+        <v>3.3490000000000002</v>
+      </c>
+      <c r="I17" s="10">
+        <v>3.3490000000000002</v>
+      </c>
+      <c r="J17" s="10">
+        <v>3.3490000000000002</v>
+      </c>
+      <c r="K17" s="10">
+        <v>3.3490000000000002</v>
+      </c>
+      <c r="L17" s="10">
+        <v>3.3490000000000002</v>
+      </c>
+      <c r="M17" s="10">
+        <v>3.3889999999999998</v>
+      </c>
+      <c r="N17" s="10">
+        <v>3.3889999999999998</v>
+      </c>
+      <c r="O17" s="10">
+        <v>3.3889999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10">
+        <v>3.4990000000000001</v>
+      </c>
+      <c r="E18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="F18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="G18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="H18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="I18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="J18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="K18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="L18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="M18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="N18" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="O18" s="11"/>
+    </row>
+    <row r="19" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="J19" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="K19" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="L19" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="M19" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="N19" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="O19" s="10">
+        <v>3.669</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3.5190000000000001</v>
+      </c>
+      <c r="D20" s="10">
+        <v>3.5190000000000001</v>
+      </c>
+      <c r="E20" s="10">
+        <v>3.5190000000000001</v>
+      </c>
+      <c r="F20" s="10">
+        <v>3.5190000000000001</v>
+      </c>
+      <c r="G20" s="10">
+        <v>3.5190000000000001</v>
+      </c>
+      <c r="H20" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="I20" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="J20" s="10">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="K20" s="10">
+        <v>3.7690000000000001</v>
+      </c>
+      <c r="L20" s="10">
+        <v>3.7690000000000001</v>
+      </c>
+      <c r="M20" s="10">
+        <v>3.7690000000000001</v>
+      </c>
+      <c r="N20" s="10">
+        <v>3.6589999999999998</v>
+      </c>
+      <c r="O20" s="11"/>
+    </row>
+    <row r="22" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="F46"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B25:D46">
+    <sortCondition ref="C25:C46"/>
+  </sortState>
+  <mergeCells count="4">
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B13:O13"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Termíno da inserção dos valores de SRS na Pesquisa #01 - Acompanhamento de valores dos postos de gasolina
</commit_message>
<xml_diff>
--- a/docs/projeto-final/documento-final/pesquisas/acompanhamento-valores.xlsx
+++ b/docs/projeto-final/documento-final/pesquisas/acompanhamento-valores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desenvolvimento\FAI\fai.etanois.docs\docs\projeto-final\documento-final\pesquisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7668F2-6E30-40B8-8A02-433F9A735C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BB59D0-947F-4131-B647-73F2181EE233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -119,16 +119,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -137,11 +131,17 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -382,6 +382,9 @@
                 <c:pt idx="13">
                   <c:v>4.859</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.859</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -529,6 +532,9 @@
                 <c:pt idx="13">
                   <c:v>5.0789999999999997</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0789999999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -820,6 +826,9 @@
                 <c:pt idx="13">
                   <c:v>5.0490000000000004</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0490000000000004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1100,6 +1109,9 @@
                   <c:v>5.149</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>5.0590000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>5.0590000000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1515,6 +1527,9 @@
                 <c:pt idx="11">
                   <c:v>3.399</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.399</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1650,6 +1665,9 @@
                 <c:pt idx="11">
                   <c:v>3.669</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.669</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1917,6 +1935,9 @@
                 <c:pt idx="11">
                   <c:v>3.5990000000000002</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2176,6 +2197,9 @@
                   <c:v>3.7690000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>3.6589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>3.6589999999999998</c:v>
                 </c:pt>
               </c:numCache>
@@ -3868,8 +3892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F419A0E-6C88-4CD1-BCBF-61ABD01E164E}">
   <dimension ref="B2:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="CO25" sqref="CO25"/>
+    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3881,64 +3905,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -4036,6 +4060,9 @@
       <c r="P6" s="3">
         <v>4.859</v>
       </c>
+      <c r="Q6" s="3">
+        <v>4.859</v>
+      </c>
     </row>
     <row r="7" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -4079,6 +4106,9 @@
         <v>5.0789999999999997</v>
       </c>
       <c r="P7" s="3">
+        <v>5.0789999999999997</v>
+      </c>
+      <c r="Q7" s="3">
         <v>5.0789999999999997</v>
       </c>
     </row>
@@ -4168,6 +4198,9 @@
         <v>5.0490000000000004</v>
       </c>
       <c r="P9" s="3">
+        <v>5.0490000000000004</v>
+      </c>
+      <c r="Q9" s="3">
         <v>5.0490000000000004</v>
       </c>
     </row>
@@ -4250,300 +4283,311 @@
       <c r="P11" s="3">
         <v>5.0590000000000002</v>
       </c>
+      <c r="Q11" s="3">
+        <v>5.0590000000000002</v>
+      </c>
     </row>
     <row r="13" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
     </row>
     <row r="14" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="6">
         <v>43836</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <v>43837</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="6">
         <v>43839</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <v>43840</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="6">
         <v>43844</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="6">
         <v>43845</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="6">
         <v>43864</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="6">
         <v>43874</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="6">
         <v>43881</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="6">
         <v>43882</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="6">
         <v>43888</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="6">
         <v>43894</v>
       </c>
-      <c r="O14" s="8">
+      <c r="O14" s="6">
         <v>43896</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8">
         <v>3.359</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="8">
         <v>3.359</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="8">
         <v>3.359</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="8">
         <v>3.359</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="8">
         <v>3.359</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="8">
         <v>3.359</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="8">
         <v>3.359</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="8">
         <v>3.399</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="8">
         <v>3.399</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="8">
         <v>3.399</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="8">
         <v>3.399</v>
       </c>
-      <c r="O15" s="11"/>
+      <c r="O15" s="8">
+        <v>3.399</v>
+      </c>
     </row>
     <row r="16" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8">
         <v>3.4590000000000001</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <v>3.4590000000000001</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="8">
         <v>3.4590000000000001</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="8">
         <v>3.669</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="8">
         <v>3.669</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="8">
         <v>3.669</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="8">
         <v>3.669</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="8">
         <v>3.669</v>
       </c>
-      <c r="O16" s="11"/>
+      <c r="O16" s="8">
+        <v>3.669</v>
+      </c>
     </row>
     <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8">
         <v>3.4590000000000001</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="8">
         <v>3.3490000000000002</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="8">
         <v>3.3490000000000002</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <v>3.3490000000000002</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="8">
         <v>3.3490000000000002</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="8">
         <v>3.3490000000000002</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="8">
         <v>3.3490000000000002</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="8">
         <v>3.3889999999999998</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="8">
         <v>3.3889999999999998</v>
       </c>
-      <c r="O17" s="10">
+      <c r="O17" s="8">
         <v>3.3889999999999998</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10">
+      <c r="C18" s="7"/>
+      <c r="D18" s="8">
         <v>3.4990000000000001</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="O18" s="11"/>
+      <c r="O18" s="8">
+        <v>3.5990000000000002</v>
+      </c>
     </row>
     <row r="19" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="10">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="O19" s="10">
+      <c r="O19" s="8">
         <v>3.669</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>3.5190000000000001</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="8">
         <v>3.5190000000000001</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="8">
         <v>3.5190000000000001</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="8">
         <v>3.5190000000000001</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="8">
         <v>3.5190000000000001</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="8">
         <v>3.5990000000000002</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="8">
         <v>3.7690000000000001</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="8">
         <v>3.7690000000000001</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="8">
         <v>3.7690000000000001</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="8">
         <v>3.6589999999999998</v>
       </c>
-      <c r="O20" s="11"/>
+      <c r="O20" s="8">
+        <v>3.6589999999999998</v>
+      </c>
     </row>
     <row r="22" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22"/>

</xml_diff>

<commit_message>
Finalização da Pesquisa #01
</commit_message>
<xml_diff>
--- a/docs/projeto-final/documento-final/pesquisas/acompanhamento-valores.xlsx
+++ b/docs/projeto-final/documento-final/pesquisas/acompanhamento-valores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desenvolvimento\FAI\fai.etanois.docs\docs\projeto-final\documento-final\pesquisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BB59D0-947F-4131-B647-73F2181EE233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC025C7-C863-4461-A233-0FB2B443E43D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
   </bookViews>
@@ -3892,8 +3892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F419A0E-6C88-4CD1-BCBF-61ABD01E164E}">
   <dimension ref="B2:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4657,56 +4657,48 @@
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
-      <c r="F31"/>
     </row>
     <row r="32" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
-      <c r="F32"/>
     </row>
     <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
-      <c r="F33"/>
     </row>
     <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
-      <c r="F34"/>
     </row>
     <row r="35" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
-      <c r="F35"/>
     </row>
     <row r="36" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
-      <c r="F36"/>
     </row>
     <row r="37" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
-      <c r="F37"/>
     </row>
     <row r="38" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
-      <c r="F38"/>
     </row>
     <row r="39" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39"/>
@@ -4760,8 +4752,8 @@
       <c r="F46"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B25:D46">
-    <sortCondition ref="C25:C46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B32:E38">
+    <sortCondition ref="C32:C38"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="B4:Q4"/>

</xml_diff>